<commit_message>
Fixed test data issue for StringConverter replacement.
</commit_message>
<xml_diff>
--- a/generic-upload-service/src/test/resources/TIS Placement Import Template - Test.xlsx
+++ b/generic-upload-service/src/test/resources/TIS Placement Import Template - Test.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yafang.deng\Documents\git\TIS-GENERIC-UPLOAD\generic-upload-service\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC46953-6391-4F7A-B134-693A6A3B1957}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Import Data" sheetId="1" r:id="rId4"/>
+    <sheet name="Import Data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="60">
   <si>
     <t>Forenames*</t>
   </si>
@@ -182,33 +191,29 @@
   </si>
   <si>
     <t>WMD/D82059/074/CT3/001</t>
+  </si>
+  <si>
+    <t>Yafang</t>
+  </si>
+  <si>
+    <t>Deng</t>
+  </si>
+  <si>
+    <t>This is for "test\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Segoe UI"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Segoe UI"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Segoe UI"/>
@@ -253,29 +258,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -284,24 +275,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -433,7 +485,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -509,7 +561,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -528,7 +580,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -558,7 +610,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -584,7 +636,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -610,7 +662,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -636,7 +688,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -662,7 +714,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -688,7 +740,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -714,7 +766,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -740,7 +792,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -766,7 +818,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -779,9 +831,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -796,7 +854,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -804,7 +862,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -823,7 +881,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -849,7 +907,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -875,7 +933,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -901,7 +959,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -927,7 +985,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -953,7 +1011,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,7 +1037,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,7 +1063,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1031,7 +1089,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1057,7 +1115,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1070,9 +1128,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1086,7 +1150,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1105,7 +1169,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1135,7 +1199,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1161,7 +1225,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1187,7 +1251,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1213,7 +1277,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1239,7 +1303,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1265,7 +1329,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1291,7 +1355,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1317,7 +1381,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1343,7 +1407,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1356,110 +1420,113 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:IV11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.6719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.8516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.8516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6719" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.3516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.3516" style="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.17188" style="1" customWidth="1"/>
+    <col min="1" max="4" width="15.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="15.6328125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="18.36328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28.453125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1796875" style="1" customWidth="1"/>
     <col min="13" max="13" width="22" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12" style="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="19.8516" style="1" customWidth="1"/>
-    <col min="18" max="18" width="23.8516" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.6719" style="1" customWidth="1"/>
-    <col min="20" max="256" width="8.85156" style="1" customWidth="1"/>
+    <col min="14" max="15" width="12" style="1" customWidth="1"/>
+    <col min="16" max="16" width="21.453125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.81640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="23.81640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6328125" style="1" customWidth="1"/>
+    <col min="20" max="256" width="8.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="2">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="2">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s" s="2">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s" s="2">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="4">
@@ -1467,48 +1534,48 @@
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" t="s" s="3">
+      <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="I2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s" s="3">
+      <c r="J2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s" s="3">
+      <c r="K2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s" s="3">
+      <c r="L2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M2" t="s" s="3">
+      <c r="M2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N2" t="s" s="3">
+      <c r="N2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O2" t="s" s="3">
+      <c r="O2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P2" t="s" s="3">
+      <c r="P2" s="3" t="s">
         <v>31</v>
       </c>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="3">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="B3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="4">
@@ -1516,48 +1583,48 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" t="s" s="3">
+      <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s" s="3">
+      <c r="G3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s" s="3">
+      <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s" s="3">
+      <c r="I3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" t="s" s="3">
+      <c r="J3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" t="s" s="3">
+      <c r="K3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L3" t="s" s="3">
+      <c r="L3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M3" t="s" s="3">
+      <c r="M3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N3" t="s" s="3">
+      <c r="N3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O3" t="s" s="3">
+      <c r="O3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P3" t="s" s="3">
+      <c r="P3" s="3" t="s">
         <v>37</v>
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="3">
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="4">
@@ -1565,48 +1632,48 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" t="s" s="3">
+      <c r="F4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G4" t="s" s="3">
+      <c r="G4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s" s="3">
+      <c r="H4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s" s="3">
+      <c r="I4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J4" t="s" s="3">
+      <c r="J4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K4" t="s" s="3">
+      <c r="K4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="s" s="3">
+      <c r="L4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M4" t="s" s="3">
+      <c r="M4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N4" t="s" s="3">
+      <c r="N4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O4" t="s" s="3">
+      <c r="O4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P4" t="s" s="3">
+      <c r="P4" s="3" t="s">
         <v>43</v>
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="3">
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s" s="3">
+      <c r="B5" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="4">
@@ -1614,48 +1681,48 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" t="s" s="3">
+      <c r="F5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G5" t="s" s="3">
+      <c r="G5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H5" t="s" s="3">
+      <c r="H5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I5" t="s" s="3">
+      <c r="I5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J5" t="s" s="3">
+      <c r="J5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K5" t="s" s="3">
+      <c r="K5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L5" t="s" s="3">
+      <c r="L5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M5" t="s" s="3">
+      <c r="M5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N5" t="s" s="3">
+      <c r="N5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O5" t="s" s="3">
+      <c r="O5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P5" t="s" s="3">
+      <c r="P5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="3">
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s" s="3">
+      <c r="B6" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="4">
@@ -1663,48 +1730,48 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" t="s" s="3">
+      <c r="F6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G6" t="s" s="3">
+      <c r="G6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H6" t="s" s="3">
+      <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I6" t="s" s="3">
+      <c r="I6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J6" t="s" s="3">
+      <c r="J6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K6" t="s" s="3">
+      <c r="K6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L6" t="s" s="3">
+      <c r="L6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M6" t="s" s="3">
+      <c r="M6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N6" t="s" s="3">
+      <c r="N6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O6" t="s" s="3">
+      <c r="O6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P6" t="s" s="3">
+      <c r="P6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="3">
+    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s" s="3">
+      <c r="B7" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="4">
@@ -1712,48 +1779,48 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" t="s" s="3">
+      <c r="F7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G7" t="s" s="3">
+      <c r="G7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H7" t="s" s="3">
+      <c r="H7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I7" t="s" s="3">
+      <c r="I7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J7" t="s" s="3">
+      <c r="J7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K7" t="s" s="3">
+      <c r="K7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L7" t="s" s="3">
+      <c r="L7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M7" t="s" s="3">
+      <c r="M7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N7" t="s" s="3">
+      <c r="N7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O7" t="s" s="3">
+      <c r="O7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P7" t="s" s="3">
+      <c r="P7" s="3" t="s">
         <v>43</v>
       </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="3">
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s" s="3">
+      <c r="B8" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="4">
@@ -1761,48 +1828,48 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" t="s" s="3">
+      <c r="F8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G8" t="s" s="3">
+      <c r="G8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H8" t="s" s="3">
+      <c r="H8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I8" t="s" s="3">
+      <c r="I8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J8" t="s" s="3">
+      <c r="J8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K8" t="s" s="3">
+      <c r="K8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L8" t="s" s="3">
+      <c r="L8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M8" t="s" s="3">
+      <c r="M8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N8" t="s" s="3">
+      <c r="N8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O8" t="s" s="3">
+      <c r="O8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P8" t="s" s="3">
+      <c r="P8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="3">
+    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s" s="3">
+      <c r="B9" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C9" s="4">
@@ -1810,48 +1877,48 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" t="s" s="3">
+      <c r="F9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G9" t="s" s="3">
+      <c r="G9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H9" t="s" s="3">
+      <c r="H9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I9" t="s" s="3">
+      <c r="I9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J9" t="s" s="3">
+      <c r="J9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K9" t="s" s="3">
+      <c r="K9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L9" t="s" s="3">
+      <c r="L9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M9" t="s" s="3">
+      <c r="M9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N9" t="s" s="3">
+      <c r="N9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O9" t="s" s="3">
+      <c r="O9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P9" t="s" s="3">
+      <c r="P9" s="3" t="s">
         <v>37</v>
       </c>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="3">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s" s="3">
+      <c r="B10" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C10" s="4">
@@ -1859,46 +1926,89 @@
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" t="s" s="3">
+      <c r="F10" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G10" t="s" s="3">
+      <c r="G10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H10" t="s" s="3">
+      <c r="H10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I10" t="s" s="3">
+      <c r="I10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J10" t="s" s="3">
+      <c r="J10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K10" t="s" s="3">
+      <c r="K10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L10" t="s" s="3">
+      <c r="L10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M10" t="s" s="3">
+      <c r="M10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N10" t="s" s="3">
+      <c r="N10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O10" t="s" s="3">
+      <c r="O10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P10" t="s" s="3">
+      <c r="P10" s="3" t="s">
         <v>43</v>
       </c>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
     </row>
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="4">
+        <v>7000019</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>